<commit_message>
Organicé el código, de nada
</commit_message>
<xml_diff>
--- a/Copia de Maya proyecto.xlsx
+++ b/Copia de Maya proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Escritorio\Documentos\Documentos universidad\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDA932E-6302-4C1E-AC26-96F36F1044DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CF0440-A8A1-4E30-ACAA-7FE013A78916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{088633CB-A06C-4593-BF05-E58B2322B816}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>Modulo</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Asignar permiso a rol</t>
   </si>
   <si>
-    <t>Actualizar rol</t>
-  </si>
-  <si>
     <t>Eliminar rol</t>
   </si>
   <si>
@@ -159,10 +156,10 @@
     <t>Crear rol</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Administrador hospital</t>
+  </si>
+  <si>
+    <t>Quitar permiso a rol</t>
   </si>
 </sst>
 </file>
@@ -264,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -569,11 +566,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -735,15 +754,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -769,6 +779,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1111,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96D9F09-A381-4083-89D3-81CC6ED406ED}">
-  <dimension ref="A1:BS61"/>
+  <dimension ref="A1:BS60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="BS34" sqref="BS34:BS61"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1153,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -1243,52 +1265,52 @@
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="63"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="36" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="37" t="s">
@@ -1311,7 +1333,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1352,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1349,7 +1371,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1390,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="60"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1387,7 +1409,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1408,7 +1430,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="67" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1423,9 +1445,9 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="58"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7" t="s">
@@ -1436,9 +1458,9 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="58"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7" t="s">
@@ -1449,32 +1471,34 @@
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="E28" s="10"/>
       <c r="F28" s="9"/>
       <c r="G28" s="13" t="s">
         <v>6</v>
@@ -1483,7 +1507,7 @@
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="56"/>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10" t="s">
@@ -1498,7 +1522,7 @@
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="56"/>
       <c r="B30" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="10" t="s">
@@ -1511,8 +1535,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="66"/>
+      <c r="B31" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="9"/>
@@ -1526,40 +1550,41 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
-      <c r="B32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="13" t="s">
+      <c r="A32" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="22" t="s">
+      <c r="A33" s="39"/>
+      <c r="B33" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="12"/>
       <c r="G33" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="BS33" s="1"/>
     </row>
     <row r="34" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="39"/>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="21"/>
@@ -1571,48 +1596,48 @@
       <c r="G34" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="BS34" s="1"/>
+      <c r="BS34" s="3"/>
     </row>
     <row r="35" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="39"/>
-      <c r="B35" s="24" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="15" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="18" t="s">
         <v>6</v>
       </c>
       <c r="BS35" s="3"/>
     </row>
     <row r="36" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="40"/>
-      <c r="B36" s="19" t="s">
+      <c r="A36" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
       <c r="BS36" s="3"/>
     </row>
     <row r="37" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="41" t="s">
-        <v>29</v>
-      </c>
+      <c r="A37" s="42"/>
       <c r="B37" s="25" t="s">
         <v>25</v>
       </c>
@@ -1645,58 +1670,58 @@
     </row>
     <row r="39" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="42"/>
-      <c r="B39" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="28"/>
+      <c r="B39" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="28"/>
       <c r="BS39" s="3"/>
     </row>
     <row r="40" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="42"/>
       <c r="B40" s="30" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="28"/>
-      <c r="BS40" s="3"/>
+      <c r="E40" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="BS40" s="6"/>
     </row>
     <row r="41" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="42"/>
-      <c r="B41" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A41" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="33"/>
+      <c r="D41" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="33"/>
+      <c r="F41" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="33"/>
       <c r="BS41" s="6"/>
     </row>
     <row r="42" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="43" t="s">
-        <v>33</v>
-      </c>
+      <c r="A42" s="44"/>
       <c r="B42" s="32" t="s">
         <v>30</v>
       </c>
@@ -1708,11 +1733,13 @@
       <c r="F42" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="33"/>
+      <c r="G42" s="34" t="s">
+        <v>6</v>
+      </c>
       <c r="BS42" s="6"/>
     </row>
     <row r="43" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="44"/>
+      <c r="A43" s="45"/>
       <c r="B43" s="32" t="s">
         <v>31</v>
       </c>
@@ -1730,22 +1757,7 @@
       <c r="BS43" s="6"/>
     </row>
     <row r="44" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="45"/>
-      <c r="B44" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="BS44" s="6"/>
+      <c r="BS44" s="9"/>
     </row>
     <row r="45" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BS45" s="9"/>
@@ -1760,7 +1772,7 @@
       <c r="BS48" s="9"/>
     </row>
     <row r="49" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS49" s="9"/>
+      <c r="BS49" s="11"/>
     </row>
     <row r="50" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BS50" s="11"/>
@@ -1769,10 +1781,10 @@
       <c r="BS51" s="11"/>
     </row>
     <row r="52" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS52" s="11"/>
+      <c r="BS52" s="16"/>
     </row>
     <row r="53" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS53" s="16"/>
+      <c r="BS53" s="28"/>
     </row>
     <row r="54" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BS54" s="28"/>
@@ -1781,35 +1793,32 @@
       <c r="BS55" s="28"/>
     </row>
     <row r="56" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS56" s="28"/>
+      <c r="BS56" s="29"/>
     </row>
     <row r="57" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BS57" s="29"/>
     </row>
     <row r="58" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS58" s="29"/>
+      <c r="BS58" s="35"/>
     </row>
     <row r="59" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS59" s="35"/>
+      <c r="BS59" s="33"/>
     </row>
     <row r="60" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BS60" s="33"/>
     </row>
-    <row r="61" spans="71:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BS61" s="33"/>
-    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A1:H11"/>
-    <mergeCell ref="A28:A32"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A18:A23"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="C15:H16"/>
+    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>